<commit_message>
Feat: estudando e aprendendo a lidar com planilhas
</commit_message>
<xml_diff>
--- a/dados/tabela_classificacao.xlsx
+++ b/dados/tabela_classificacao.xlsx
@@ -626,10 +626,10 @@
         <v>10</v>
       </c>
       <c r="G6" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="H6" t="n">
-        <v>-10</v>
+        <v>5</v>
       </c>
       <c r="I6" t="n">
         <v>13</v>

</xml_diff>